<commit_message>
Add import/export cost/revenue to objective function
Fix definition of pImpExpPrice to be parameter
</commit_message>
<xml_diff>
--- a/data/example/Power_ImpExp.xlsx
+++ b/data/example/Power_ImpExp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95726145-DF84-4F39-BB07-78CB718B53A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F969C4-B5EB-455B-ADC3-404C38F678F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34572" yWindow="-17508" windowWidth="30936" windowHeight="16776" tabRatio="857" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -883,7 +883,9 @@
   </sheetPr>
   <dimension ref="B1:AB27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>